<commit_message>
Updated presentations and requirements xref.
</commit_message>
<xml_diff>
--- a/Requirements Xref Matrix.xlsx
+++ b/Requirements Xref Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="20115" windowHeight="6210" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="20115" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Attachment A" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <definedName name="Attachment_C" localSheetId="2">'Attachment C'!$B$2:$D$12</definedName>
     <definedName name="Scheduling_ONLY_Table_INFO" localSheetId="0">'Attachment A'!$B$1:$D$128</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="304">
   <si>
     <t>Attachment A--Scheduling</t>
   </si>
@@ -900,6 +900,63 @@
   <si>
     <t>The system shall associate each appointment type with the correct DSS stop code/ credit stop; see:
 http://www1.va.gov/vhapublications/ViewPublication.asp?pub_ID=1788 788</t>
+  </si>
+  <si>
+    <t>OpenMash Vision</t>
+  </si>
+  <si>
+    <t>The RPC and CIA adaptors extends the reach of the current MedSphere remote procedure calls to all existing VistA clients.  Additional integration concerns can be transparently layered on top.</t>
+  </si>
+  <si>
+    <t>ESB provides ErrorHandling and Exception handling with Apache Camel.  Exception handling flexibly identifies error handling routes based on Exception hierarchy.  Dead-letter-queue pattern is supported.  Error handling can be added  as flexible interceptors with scope at the context, RouteBuilder, or route scope.  Interceptor pattern means error handling does not obscure primary workflow design.</t>
+  </si>
+  <si>
+    <t>Transport mediation is handle by ESB.  With the RPC and CIA transport adaptors, a bridge is created that extends VistA's reach with any supported transport, including but not limited to SOAP/HTTP, SOAP/JMS, REST, ftp, etc.</t>
+  </si>
+  <si>
+    <t>Provided by MedSphere.  The ESB RPC adaptors ensures that this is bidirection, i.e. other apps will be able to leverage MedSphere scheduling remote procedures and vice versa.</t>
+  </si>
+  <si>
+    <t>Provided by ESB.  HTTPS, SSL/TLS, FTPS and SFTP, and many other secure transports are supported.  In addition, message layer security is also supported using open standards such WS-Security.</t>
+  </si>
+  <si>
+    <t>Medsphere Scheduling client.</t>
+  </si>
+  <si>
+    <t>Handled by MedSphere Scheduling Client app.</t>
+  </si>
+  <si>
+    <t>The MedSphere Scheduling client is a .NET application, but can potentially be ported to mono for  Linux.  All of the additional infrastructure will run on linux or windows.  The Google App Engine, Cosmo UI, Syncope, and other user interfaces can run in the browser.</t>
+  </si>
+  <si>
+    <t>This is provided OTB via the wire-tap pattern demonstrated in the VistA-HL7 integration example.</t>
+  </si>
+  <si>
+    <t>Yes, highly modular development environment allows just about anything to be isolated, mocked, refactored, and then extended.  See the Developers Guide for individual level support.  See the Vista-HL7 integration case for an example of how just about anything can be mocked.</t>
+  </si>
+  <si>
+    <t>This is done today with MedSphere, but in the future it can be done with Standards such as iCal and CalDav.  The Cosmo Server is an option for an OSS standards compliant scheduling engine.  The Google Calendar is an example of integrating that with SaaS.  Note the additional Google Documents with respect to various certification and security levels.</t>
+  </si>
+  <si>
+    <t>MedSphere Scheduling Client.</t>
+  </si>
+  <si>
+    <t>Yes, see Vista-HL for an example of the wire-tap and store pattern.  The same pattern can be applied to any service, including configuration services for resources.</t>
+  </si>
+  <si>
+    <t>Routing rules can be dynamically modified in the ESB.  The ESB supports integration with business rules engines such as Drools.  Similar examples are documented in Mirth.</t>
+  </si>
+  <si>
+    <t>Yes.  This comes through integration based on standards.  Any iCal compatible device can do this.  Google has many such vendors available in its marketplace already.</t>
+  </si>
+  <si>
+    <t>See MedSphere Client, Cosmo UI Client, Google UI.</t>
+  </si>
+  <si>
+    <t>Yes, see MedSphere Client, Cosmo UI Client, Google UI.</t>
+  </si>
+  <si>
+    <t>Yes, see MedSphere Client, Cosmo UI Client, Google UI.  This is demonstrated in the Volunteer Ride Share demo where both scheduling windows and geography and mashed together to match volunteers with patients.  The same algorithms can be used to match other things such as resources and patients, or providers and resources.</t>
   </si>
 </sst>
 </file>
@@ -958,7 +1015,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1007,6 +1064,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1317,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D128"/>
+  <dimension ref="B1:E128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,17 +1392,18 @@
     <col min="2" max="2" width="34.140625" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="81.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
@@ -1349,8 +1413,11 @@
       <c r="D3" s="11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="E3" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="150" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>206</v>
       </c>
@@ -1360,8 +1427,11 @@
       <c r="D4" s="9" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E4" s="19" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="165" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="8">
         <v>1.2</v>
@@ -1369,8 +1439,11 @@
       <c r="D5" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E5" s="19" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="8" t="s">
         <v>2</v>
@@ -1378,8 +1451,11 @@
       <c r="D6" s="9" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E6" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="8" t="s">
         <v>3</v>
@@ -1387,8 +1463,11 @@
       <c r="D7" s="9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E7" s="19" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="8" t="s">
         <v>4</v>
@@ -1396,8 +1475,11 @@
       <c r="D8" s="9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E8" s="19" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="8" t="s">
         <v>5</v>
@@ -1405,8 +1487,11 @@
       <c r="D9" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E9" s="19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
         <v>6</v>
@@ -1414,8 +1499,11 @@
       <c r="D10" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E10" s="19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="8">
         <v>1.3</v>
@@ -1423,8 +1511,11 @@
       <c r="D11" s="9" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E11" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="8" t="s">
         <v>7</v>
@@ -1432,8 +1523,11 @@
       <c r="D12" s="9" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E12" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="8" t="s">
         <v>8</v>
@@ -1441,8 +1535,11 @@
       <c r="D13" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E13" s="19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="8" t="s">
         <v>9</v>
@@ -1450,8 +1547,11 @@
       <c r="D14" s="9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E14" s="19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="8" t="s">
         <v>10</v>
@@ -1459,8 +1559,11 @@
       <c r="D15" s="9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E15" s="19" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="8" t="s">
         <v>11</v>
@@ -1468,8 +1571,11 @@
       <c r="D16" s="9" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E16" s="19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
         <v>12</v>
@@ -1477,8 +1583,9 @@
       <c r="D17" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E17" s="19"/>
+    </row>
+    <row r="18" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
         <v>13</v>
@@ -1486,8 +1593,9 @@
       <c r="D18" s="9" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="8">
         <v>1.4</v>
@@ -1495,8 +1603,9 @@
       <c r="D19" s="9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="8" t="s">
         <v>14</v>
@@ -1504,8 +1613,9 @@
       <c r="D20" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E20" s="19"/>
+    </row>
+    <row r="21" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="8" t="s">
         <v>15</v>
@@ -1513,8 +1623,9 @@
       <c r="D21" s="9" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="8" t="s">
         <v>16</v>
@@ -1522,8 +1633,9 @@
       <c r="D22" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="8" t="s">
         <v>17</v>
@@ -1531,8 +1643,9 @@
       <c r="D23" s="9" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E23" s="19"/>
+    </row>
+    <row r="24" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="8" t="s">
         <v>18</v>
@@ -1540,8 +1653,9 @@
       <c r="D24" s="9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E24" s="19"/>
+    </row>
+    <row r="25" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="8">
         <v>1.5</v>
@@ -1549,8 +1663,9 @@
       <c r="D25" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="8">
         <v>1.6</v>
@@ -1558,8 +1673,9 @@
       <c r="D26" s="9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E26" s="19"/>
+    </row>
+    <row r="27" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
         <v>19</v>
@@ -1567,8 +1683,9 @@
       <c r="D27" s="9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E27" s="19"/>
+    </row>
+    <row r="28" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="8">
         <v>1.7</v>
@@ -1576,8 +1693,9 @@
       <c r="D28" s="9" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E28" s="19"/>
+    </row>
+    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="8" t="s">
         <v>20</v>
@@ -1585,8 +1703,9 @@
       <c r="D29" s="9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E29" s="19"/>
+    </row>
+    <row r="30" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="8" t="s">
         <v>21</v>
@@ -1594,8 +1713,9 @@
       <c r="D30" s="9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E30" s="19"/>
+    </row>
+    <row r="31" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>207</v>
       </c>
@@ -1605,8 +1725,9 @@
       <c r="D31" s="9" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E31" s="19"/>
+    </row>
+    <row r="32" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="8">
         <v>2.2000000000000002</v>
@@ -1614,8 +1735,9 @@
       <c r="D32" s="9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E32" s="19"/>
+    </row>
+    <row r="33" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="8">
         <v>2.2999999999999998</v>
@@ -1623,8 +1745,9 @@
       <c r="D33" s="9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E33" s="19"/>
+    </row>
+    <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="8">
         <v>2.4</v>
@@ -1632,8 +1755,9 @@
       <c r="D34" s="9" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="2:5" ht="150" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="8">
         <v>2.5</v>
@@ -1641,8 +1765,9 @@
       <c r="D35" s="9" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E35" s="19"/>
+    </row>
+    <row r="36" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="8">
         <v>2.6</v>
@@ -1650,8 +1775,9 @@
       <c r="D36" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E36" s="19"/>
+    </row>
+    <row r="37" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="8">
         <v>2.7</v>
@@ -1659,8 +1785,9 @@
       <c r="D37" s="9" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E37" s="19"/>
+    </row>
+    <row r="38" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="8">
         <v>2.8</v>
@@ -1668,8 +1795,9 @@
       <c r="D38" s="9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" ht="330" x14ac:dyDescent="0.25">
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="2:5" ht="330" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>208</v>
       </c>
@@ -1679,8 +1807,9 @@
       <c r="D39" s="9" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E39" s="19"/>
+    </row>
+    <row r="40" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="8" t="s">
         <v>22</v>
@@ -1688,8 +1817,9 @@
       <c r="D40" s="9" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E40" s="19"/>
+    </row>
+    <row r="41" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="8" t="s">
         <v>23</v>
@@ -1697,8 +1827,9 @@
       <c r="D41" s="9" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E41" s="19"/>
+    </row>
+    <row r="42" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="C42" s="8" t="s">
         <v>24</v>
@@ -1706,8 +1837,9 @@
       <c r="D42" s="9" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E42" s="19"/>
+    </row>
+    <row r="43" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="C43" s="8" t="s">
         <v>25</v>
@@ -1715,8 +1847,9 @@
       <c r="D43" s="9" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E43" s="19"/>
+    </row>
+    <row r="44" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="C44" s="8">
         <v>3.2</v>
@@ -1724,8 +1857,9 @@
       <c r="D44" s="9" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E44" s="19"/>
+    </row>
+    <row r="45" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
       <c r="C45" s="8">
         <v>3.3</v>
@@ -1733,8 +1867,9 @@
       <c r="D45" s="9" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E45" s="19"/>
+    </row>
+    <row r="46" spans="2:5" ht="165" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="C46" s="8">
         <v>3.4</v>
@@ -1742,8 +1877,9 @@
       <c r="D46" s="9" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E46" s="19"/>
+    </row>
+    <row r="47" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
       <c r="C47" s="8">
         <v>3.5</v>
@@ -1751,8 +1887,9 @@
       <c r="D47" s="9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E47" s="19"/>
+    </row>
+    <row r="48" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" s="8" t="s">
         <v>26</v>
@@ -1760,8 +1897,9 @@
       <c r="D48" s="9" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E48" s="19"/>
+    </row>
+    <row r="49" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" s="8" t="s">
         <v>27</v>
@@ -1769,8 +1907,9 @@
       <c r="D49" s="9" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E49" s="19"/>
+    </row>
+    <row r="50" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="8" t="s">
         <v>28</v>
@@ -1778,8 +1917,9 @@
       <c r="D50" s="9" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E50" s="19"/>
+    </row>
+    <row r="51" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
       <c r="C51" s="8" t="s">
         <v>29</v>
@@ -1787,8 +1927,9 @@
       <c r="D51" s="9" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E51" s="19"/>
+    </row>
+    <row r="52" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="C52" s="8" t="s">
         <v>30</v>
@@ -1796,8 +1937,9 @@
       <c r="D52" s="9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E52" s="19"/>
+    </row>
+    <row r="53" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B53" s="7"/>
       <c r="C53" s="8">
         <v>3.6</v>
@@ -1805,8 +1947,9 @@
       <c r="D53" s="9" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E53" s="19"/>
+    </row>
+    <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="C54" s="8" t="s">
         <v>31</v>
@@ -1814,8 +1957,9 @@
       <c r="D54" s="9" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E54" s="19"/>
+    </row>
+    <row r="55" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
       <c r="C55" s="8" t="s">
         <v>32</v>
@@ -1823,8 +1967,9 @@
       <c r="D55" s="9" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E55" s="19"/>
+    </row>
+    <row r="56" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="C56" s="8" t="s">
         <v>33</v>
@@ -1832,8 +1977,9 @@
       <c r="D56" s="9" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E56" s="19"/>
+    </row>
+    <row r="57" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
       <c r="C57" s="8" t="s">
         <v>34</v>
@@ -1841,8 +1987,9 @@
       <c r="D57" s="9" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E57" s="19"/>
+    </row>
+    <row r="58" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
       <c r="C58" s="8" t="s">
         <v>35</v>
@@ -1850,8 +1997,9 @@
       <c r="D58" s="9" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="59" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E58" s="19"/>
+    </row>
+    <row r="59" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
       <c r="C59" s="8">
         <v>3.7</v>
@@ -1859,8 +2007,9 @@
       <c r="D59" s="9" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E59" s="19"/>
+    </row>
+    <row r="60" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
       <c r="C60" s="8" t="s">
         <v>36</v>
@@ -1868,8 +2017,9 @@
       <c r="D60" s="9" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E60" s="19"/>
+    </row>
+    <row r="61" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
       <c r="C61" s="8" t="s">
         <v>37</v>
@@ -1877,8 +2027,9 @@
       <c r="D61" s="9" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E61" s="19"/>
+    </row>
+    <row r="62" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B62" s="7"/>
       <c r="C62" s="8" t="s">
         <v>38</v>
@@ -1886,8 +2037,9 @@
       <c r="D62" s="9" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E62" s="19"/>
+    </row>
+    <row r="63" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
       <c r="C63" s="8" t="s">
         <v>39</v>
@@ -1895,8 +2047,9 @@
       <c r="D63" s="9" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="64" spans="2:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E63" s="19"/>
+    </row>
+    <row r="64" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
       <c r="C64" s="8" t="s">
         <v>40</v>
@@ -1904,8 +2057,9 @@
       <c r="D64" s="9" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E64" s="19"/>
+    </row>
+    <row r="65" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
       <c r="C65" s="8" t="s">
         <v>41</v>
@@ -1913,8 +2067,9 @@
       <c r="D65" s="9" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E65" s="19"/>
+    </row>
+    <row r="66" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B66" s="7"/>
       <c r="C66" s="8">
         <v>3.8</v>
@@ -1922,8 +2077,9 @@
       <c r="D66" s="9" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E66" s="19"/>
+    </row>
+    <row r="67" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B67" s="7"/>
       <c r="C67" s="8" t="s">
         <v>42</v>
@@ -1931,8 +2087,9 @@
       <c r="D67" s="9" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E67" s="19"/>
+    </row>
+    <row r="68" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B68" s="7"/>
       <c r="C68" s="8" t="s">
         <v>43</v>
@@ -1940,8 +2097,9 @@
       <c r="D68" s="9" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E68" s="19"/>
+    </row>
+    <row r="69" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B69" s="7"/>
       <c r="C69" s="8" t="s">
         <v>44</v>
@@ -1949,8 +2107,9 @@
       <c r="D69" s="9" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E69" s="19"/>
+    </row>
+    <row r="70" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
         <v>209</v>
       </c>
@@ -1960,8 +2119,9 @@
       <c r="D70" s="9" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E70" s="19"/>
+    </row>
+    <row r="71" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B71" s="7"/>
       <c r="C71" s="8" t="s">
         <v>45</v>
@@ -1969,8 +2129,9 @@
       <c r="D71" s="9" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E71" s="19"/>
+    </row>
+    <row r="72" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B72" s="7"/>
       <c r="C72" s="8" t="s">
         <v>46</v>
@@ -1978,8 +2139,9 @@
       <c r="D72" s="9" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="73" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E72" s="19"/>
+    </row>
+    <row r="73" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B73" s="7"/>
       <c r="C73" s="8" t="s">
         <v>47</v>
@@ -1987,8 +2149,9 @@
       <c r="D73" s="9" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="74" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E73" s="19"/>
+    </row>
+    <row r="74" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B74" s="7"/>
       <c r="C74" s="8" t="s">
         <v>48</v>
@@ -1996,8 +2159,9 @@
       <c r="D74" s="9" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="75" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E74" s="19"/>
+    </row>
+    <row r="75" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B75" s="7"/>
       <c r="C75" s="8" t="s">
         <v>49</v>
@@ -2005,8 +2169,9 @@
       <c r="D75" s="9" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="76" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E75" s="19"/>
+    </row>
+    <row r="76" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B76" s="7"/>
       <c r="C76" s="8" t="s">
         <v>50</v>
@@ -2014,8 +2179,9 @@
       <c r="D76" s="9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="77" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E76" s="19"/>
+    </row>
+    <row r="77" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B77" s="7"/>
       <c r="C77" s="8" t="s">
         <v>51</v>
@@ -2023,8 +2189,9 @@
       <c r="D77" s="9" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="78" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E77" s="19"/>
+    </row>
+    <row r="78" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
       <c r="C78" s="8">
         <v>4.2</v>
@@ -2032,8 +2199,9 @@
       <c r="D78" s="9" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="79" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E78" s="19"/>
+    </row>
+    <row r="79" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B79" s="7"/>
       <c r="C79" s="8" t="s">
         <v>52</v>
@@ -2041,8 +2209,9 @@
       <c r="D79" s="9" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="80" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E79" s="19"/>
+    </row>
+    <row r="80" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
       <c r="C80" s="8" t="s">
         <v>53</v>
@@ -2050,8 +2219,9 @@
       <c r="D80" s="9" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="81" spans="2:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="E80" s="19"/>
+    </row>
+    <row r="81" spans="2:5" ht="150" x14ac:dyDescent="0.25">
       <c r="B81" s="7"/>
       <c r="C81" s="8" t="s">
         <v>54</v>
@@ -2059,8 +2229,9 @@
       <c r="D81" s="9" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="82" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E81" s="19"/>
+    </row>
+    <row r="82" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B82" s="7"/>
       <c r="C82" s="8" t="s">
         <v>55</v>
@@ -2068,8 +2239,9 @@
       <c r="D82" s="9" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="83" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E82" s="19"/>
+    </row>
+    <row r="83" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B83" s="7"/>
       <c r="C83" s="8" t="s">
         <v>56</v>
@@ -2077,8 +2249,9 @@
       <c r="D83" s="9" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="84" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E83" s="19"/>
+    </row>
+    <row r="84" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B84" s="7"/>
       <c r="C84" s="8" t="s">
         <v>57</v>
@@ -2086,8 +2259,9 @@
       <c r="D84" s="9" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="85" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E84" s="19"/>
+    </row>
+    <row r="85" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B85" s="7"/>
       <c r="C85" s="8" t="s">
         <v>58</v>
@@ -2095,8 +2269,9 @@
       <c r="D85" s="9" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="86" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E85" s="19"/>
+    </row>
+    <row r="86" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B86" s="7"/>
       <c r="C86" s="8">
         <v>4.3</v>
@@ -2104,8 +2279,9 @@
       <c r="D86" s="9" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="87" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E86" s="19"/>
+    </row>
+    <row r="87" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B87" s="7"/>
       <c r="C87" s="8" t="s">
         <v>59</v>
@@ -2113,8 +2289,9 @@
       <c r="D87" s="9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="88" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E87" s="19"/>
+    </row>
+    <row r="88" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B88" s="7"/>
       <c r="C88" s="8" t="s">
         <v>60</v>
@@ -2122,8 +2299,9 @@
       <c r="D88" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="89" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E88" s="19"/>
+    </row>
+    <row r="89" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B89" s="7"/>
       <c r="C89" s="8" t="s">
         <v>61</v>
@@ -2131,8 +2309,9 @@
       <c r="D89" s="9" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="90" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E89" s="19"/>
+    </row>
+    <row r="90" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B90" s="7"/>
       <c r="C90" s="8" t="s">
         <v>62</v>
@@ -2140,8 +2319,9 @@
       <c r="D90" s="9" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="91" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E90" s="19"/>
+    </row>
+    <row r="91" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B91" s="7"/>
       <c r="C91" s="8" t="s">
         <v>63</v>
@@ -2149,8 +2329,9 @@
       <c r="D91" s="9" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="92" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E91" s="19"/>
+    </row>
+    <row r="92" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B92" s="7"/>
       <c r="C92" s="8" t="s">
         <v>64</v>
@@ -2158,8 +2339,9 @@
       <c r="D92" s="9" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="93" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E92" s="19"/>
+    </row>
+    <row r="93" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B93" s="7"/>
       <c r="C93" s="8">
         <v>4.4000000000000004</v>
@@ -2167,8 +2349,9 @@
       <c r="D93" s="9" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="94" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E93" s="19"/>
+    </row>
+    <row r="94" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B94" s="7"/>
       <c r="C94" s="8" t="s">
         <v>65</v>
@@ -2176,8 +2359,9 @@
       <c r="D94" s="9" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="95" spans="2:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E94" s="19"/>
+    </row>
+    <row r="95" spans="2:5" ht="165" x14ac:dyDescent="0.25">
       <c r="B95" s="7"/>
       <c r="C95" s="8" t="s">
         <v>66</v>
@@ -2185,8 +2369,9 @@
       <c r="D95" s="9" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="96" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E95" s="19"/>
+    </row>
+    <row r="96" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B96" s="7"/>
       <c r="C96" s="8" t="s">
         <v>67</v>
@@ -2194,8 +2379,9 @@
       <c r="D96" s="9" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="97" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E96" s="19"/>
+    </row>
+    <row r="97" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B97" s="7"/>
       <c r="C97" s="8" t="s">
         <v>68</v>
@@ -2203,8 +2389,9 @@
       <c r="D97" s="9" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="98" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E97" s="19"/>
+    </row>
+    <row r="98" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B98" s="7"/>
       <c r="C98" s="8" t="s">
         <v>69</v>
@@ -2212,8 +2399,9 @@
       <c r="D98" s="9" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="99" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E98" s="19"/>
+    </row>
+    <row r="99" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B99" s="4" t="s">
         <v>210</v>
       </c>
@@ -2223,8 +2411,9 @@
       <c r="D99" s="9" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="100" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E99" s="19"/>
+    </row>
+    <row r="100" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B100" s="7"/>
       <c r="C100" s="8" t="s">
         <v>70</v>
@@ -2232,8 +2421,9 @@
       <c r="D100" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="101" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E100" s="19"/>
+    </row>
+    <row r="101" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B101" s="7"/>
       <c r="C101" s="8" t="s">
         <v>71</v>
@@ -2241,8 +2431,9 @@
       <c r="D101" s="9" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="102" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E101" s="19"/>
+    </row>
+    <row r="102" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B102" s="7"/>
       <c r="C102" s="8" t="s">
         <v>72</v>
@@ -2250,8 +2441,9 @@
       <c r="D102" s="9" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="103" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E102" s="19"/>
+    </row>
+    <row r="103" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B103" s="7"/>
       <c r="C103" s="8">
         <v>5.2</v>
@@ -2259,8 +2451,9 @@
       <c r="D103" s="9" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="104" spans="2:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E103" s="19"/>
+    </row>
+    <row r="104" spans="2:5" ht="165" x14ac:dyDescent="0.25">
       <c r="B104" s="7"/>
       <c r="C104" s="8" t="s">
         <v>73</v>
@@ -2268,8 +2461,9 @@
       <c r="D104" s="9" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="105" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E104" s="19"/>
+    </row>
+    <row r="105" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
       <c r="C105" s="8" t="s">
         <v>74</v>
@@ -2277,8 +2471,9 @@
       <c r="D105" s="9" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="106" spans="2:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E105" s="19"/>
+    </row>
+    <row r="106" spans="2:5" ht="165" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
       <c r="C106" s="8" t="s">
         <v>75</v>
@@ -2286,8 +2481,9 @@
       <c r="D106" s="9" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="107" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E106" s="19"/>
+    </row>
+    <row r="107" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B107" s="7"/>
       <c r="C107" s="8" t="s">
         <v>76</v>
@@ -2295,8 +2491,9 @@
       <c r="D107" s="9" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="108" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E107" s="19"/>
+    </row>
+    <row r="108" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B108" s="7"/>
       <c r="C108" s="8">
         <v>5.3</v>
@@ -2304,8 +2501,9 @@
       <c r="D108" s="9" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="109" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E108" s="19"/>
+    </row>
+    <row r="109" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B109" s="7"/>
       <c r="C109" s="8" t="s">
         <v>77</v>
@@ -2313,8 +2511,9 @@
       <c r="D109" s="9" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="110" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E109" s="19"/>
+    </row>
+    <row r="110" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B110" s="7"/>
       <c r="C110" s="8" t="s">
         <v>78</v>
@@ -2322,8 +2521,9 @@
       <c r="D110" s="9" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="111" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E110" s="19"/>
+    </row>
+    <row r="111" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B111" s="7"/>
       <c r="C111" s="8" t="s">
         <v>79</v>
@@ -2331,8 +2531,9 @@
       <c r="D111" s="9" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="112" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E111" s="19"/>
+    </row>
+    <row r="112" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B112" s="7"/>
       <c r="C112" s="8" t="s">
         <v>80</v>
@@ -2340,8 +2541,9 @@
       <c r="D112" s="9" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="113" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E112" s="19"/>
+    </row>
+    <row r="113" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B113" s="7"/>
       <c r="C113" s="8">
         <v>5.4</v>
@@ -2349,8 +2551,9 @@
       <c r="D113" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="114" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E113" s="19"/>
+    </row>
+    <row r="114" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B114" s="4" t="s">
         <v>211</v>
       </c>
@@ -2360,8 +2563,9 @@
       <c r="D114" s="9" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="115" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E114" s="19"/>
+    </row>
+    <row r="115" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B115" s="7"/>
       <c r="C115" s="8">
         <v>6.2</v>
@@ -2369,8 +2573,9 @@
       <c r="D115" s="9" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="116" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E115" s="19"/>
+    </row>
+    <row r="116" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B116" s="7"/>
       <c r="C116" s="8">
         <v>6.3</v>
@@ -2378,8 +2583,9 @@
       <c r="D116" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="117" spans="2:4" ht="255" x14ac:dyDescent="0.25">
+      <c r="E116" s="19"/>
+    </row>
+    <row r="117" spans="2:5" ht="255" x14ac:dyDescent="0.25">
       <c r="B117" s="4" t="s">
         <v>212</v>
       </c>
@@ -2389,8 +2595,9 @@
       <c r="D117" s="9" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="118" spans="2:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="E117" s="19"/>
+    </row>
+    <row r="118" spans="2:5" ht="150" x14ac:dyDescent="0.25">
       <c r="B118" s="7"/>
       <c r="C118" s="8" t="s">
         <v>81</v>
@@ -2398,8 +2605,9 @@
       <c r="D118" s="9" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="119" spans="2:4" ht="240" x14ac:dyDescent="0.25">
+      <c r="E118" s="19"/>
+    </row>
+    <row r="119" spans="2:5" ht="240" x14ac:dyDescent="0.25">
       <c r="B119" s="7"/>
       <c r="C119" s="8" t="s">
         <v>82</v>
@@ -2407,8 +2615,9 @@
       <c r="D119" s="9" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="120" spans="2:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E119" s="19"/>
+    </row>
+    <row r="120" spans="2:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B120" s="7"/>
       <c r="C120" s="8" t="s">
         <v>83</v>
@@ -2416,8 +2625,9 @@
       <c r="D120" s="9" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="121" spans="2:4" ht="270" x14ac:dyDescent="0.25">
+      <c r="E120" s="19"/>
+    </row>
+    <row r="121" spans="2:5" ht="270" x14ac:dyDescent="0.25">
       <c r="B121" s="7"/>
       <c r="C121" s="8">
         <v>7.2</v>
@@ -2425,8 +2635,9 @@
       <c r="D121" s="9" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="122" spans="2:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="E121" s="19"/>
+    </row>
+    <row r="122" spans="2:5" ht="195" x14ac:dyDescent="0.25">
       <c r="B122" s="7"/>
       <c r="C122" s="8" t="s">
         <v>84</v>
@@ -2434,24 +2645,25 @@
       <c r="D122" s="9" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="19"/>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D124" s="1"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D125" s="1"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D126" s="1"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C127" s="3"/>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D128" s="1"/>
     </row>
   </sheetData>
@@ -2465,7 +2677,7 @@
   <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2832,10 +3044,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D12"/>
+  <dimension ref="B1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2843,14 +3055,15 @@
     <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>263</v>
       </c>
@@ -2860,8 +3073,11 @@
       <c r="D3" s="10" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E3" s="20" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>266</v>
       </c>
@@ -2869,8 +3085,11 @@
       <c r="D4" s="18" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E4" s="19" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="16" t="s">
         <v>267</v>
@@ -2878,8 +3097,11 @@
       <c r="D5" s="18" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E5" s="19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="16" t="s">
         <v>268</v>
@@ -2887,15 +3109,21 @@
       <c r="D6" s="18" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E6" s="19" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="18" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E7" s="19" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="16" t="s">
         <v>269</v>
@@ -2903,8 +3131,11 @@
       <c r="D8" s="18" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="E8" s="19" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="195" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>270</v>
       </c>
@@ -2914,15 +3145,21 @@
       <c r="D9" s="18" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E9" s="19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E10" s="19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>272</v>
       </c>
@@ -2932,14 +3169,20 @@
       <c r="D11" s="18" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E11" s="19" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
       <c r="C12" s="16" t="s">
         <v>274</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>283</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>